<commit_message>
SIMPLEX-64 Custom concept sheet branch time check.
</commit_message>
<xml_diff>
--- a/api/src/test/resources/test-spreadsheets/conceptsSpreadsheet.xlsx
+++ b/api/src/test/resources/test-spreadsheets/conceptsSpreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/c/simple-extension-toolkit/api/src/test/resources/test-spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94C7E43-0923-2145-BD04-88DB16228FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B1964D-F74B-2643-85D8-B50A9057ACFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,13 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="45">
   <si>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Parent Concept Identifier</t>
     </r>
@@ -58,6 +59,7 @@
         <b/>
         <sz val="11"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Parent Concept Term</t>
     </r>
@@ -89,6 +91,7 @@
         <b/>
         <sz val="11"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Concept Identifier</t>
     </r>
@@ -121,6 +124,7 @@
         <b/>
         <sz val="11"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Active</t>
     </r>
@@ -153,6 +157,7 @@
         <b/>
         <sz val="11"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Terms in English, US dialect</t>
     </r>
@@ -185,6 +190,7 @@
         <b/>
         <sz val="11"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Terms in My translation (214916581000003106)</t>
     </r>
@@ -328,6 +334,7 @@
         <b/>
         <sz val="11"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Terms in Some language reference set (971232511000003100)</t>
     </r>
@@ -343,6 +350,9 @@
 The first term will be the preferred term. 
 Each additional synonym should use a new row. There is no need to repeat the values in columns A to D.</t>
     </r>
+  </si>
+  <si>
+    <t>Simplex branch timestamp:1727964880378</t>
   </si>
 </sst>
 </file>
@@ -361,6 +371,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -725,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:CA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="BA1" workbookViewId="0">
+      <selection activeCell="BN10" sqref="BN10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -740,7 +751,7 @@
     <col min="5" max="7" width="58.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:79" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -762,8 +773,11 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="CA1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -786,7 +800,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -809,7 +823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:79" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -832,7 +846,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -855,7 +869,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F6" s="2" t="s">
         <v>9</v>
       </c>
@@ -863,7 +877,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -882,7 +896,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -905,7 +919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E9" s="2" t="s">
         <v>29</v>
       </c>
@@ -916,7 +930,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -939,7 +953,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:79" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -962,7 +976,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -985,7 +999,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1008,7 +1022,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:79" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>

</xml_diff>